<commit_message>
the fight ui design is complete but the panel's size is can't change with the widget
</commit_message>
<xml_diff>
--- a/source/竞技对战表/竞技输入格式1--2025-5-1--zhou .xlsx
+++ b/source/竞技对战表/竞技输入格式1--2025-5-1--zhou .xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\bieren\taekwondo\WTF-Trans\WTF\source\竞技对战表\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3865621E-5220-4DA9-94B4-BE38AFFE9BD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="120" windowWidth="14376" windowHeight="11640"/>
+    <workbookView xWindow="25510" yWindow="0" windowWidth="12980" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -831,7 +837,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -934,14 +940,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -955,6 +955,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -965,14 +971,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1010,7 +1019,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1082,7 +1091,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1255,88 +1264,88 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J794"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K16" sqref="K16"/>
+      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="6.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" style="2" customWidth="1"/>
+    <col min="1" max="2" width="6.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.54296875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="10" style="2" customWidth="1"/>
-    <col min="6" max="6" width="4.77734375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.77734375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="4.81640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.81640625" style="2" customWidth="1"/>
     <col min="8" max="8" width="10" style="2" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="7.5546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="15.08984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.54296875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="3" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-    </row>
-    <row r="2" spans="1:10" s="5" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+    </row>
+    <row r="2" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-    </row>
-    <row r="3" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+    </row>
+    <row r="3" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7" t="s">
+      <c r="F3" s="5"/>
+      <c r="G3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -1358,11 +1367,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+    <row r="5" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -1384,11 +1393,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -1410,11 +1419,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+    <row r="7" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -1436,11 +1445,11 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+    <row r="8" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -1462,11 +1471,11 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+    <row r="9" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -1488,11 +1497,11 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+    <row r="10" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -1514,11 +1523,11 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+    <row r="11" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -1540,11 +1549,11 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+    <row r="12" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -1566,11 +1575,11 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+    <row r="13" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -1592,11 +1601,11 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+    <row r="14" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -1618,11 +1627,11 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+    <row r="15" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D15" s="2" t="s">
@@ -1644,11 +1653,11 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+    <row r="16" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="2" t="s">
@@ -1670,11 +1679,11 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+    <row r="17" spans="1:9" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -1696,11 +1705,11 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
+    <row r="18" spans="1:9" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -1722,11 +1731,11 @@
         <v>71</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
+    <row r="19" spans="1:9" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="8" t="s">
         <v>73</v>
       </c>
       <c r="D19" s="2" t="s">
@@ -1745,11 +1754,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
+    <row r="20" spans="1:9" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="8" t="s">
         <v>73</v>
       </c>
       <c r="D20" s="2" t="s">
@@ -1765,11 +1774,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
+    <row r="21" spans="1:9" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="8" t="s">
         <v>73</v>
       </c>
       <c r="D21" s="2" t="s">
@@ -1788,11 +1797,11 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+    <row r="22" spans="1:9" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="8" t="s">
         <v>73</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -1808,11 +1817,11 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
+    <row r="23" spans="1:9" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="8" t="s">
         <v>73</v>
       </c>
       <c r="D23" s="2" t="s">
@@ -1831,11 +1840,11 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
+    <row r="24" spans="1:9" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="8" t="s">
         <v>73</v>
       </c>
       <c r="D24" s="2" t="s">
@@ -1854,11 +1863,11 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
+    <row r="25" spans="1:9" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="8" t="s">
         <v>73</v>
       </c>
       <c r="D25" s="2" t="s">
@@ -1877,11 +1886,11 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
+    <row r="26" spans="1:9" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="8" t="s">
         <v>73</v>
       </c>
       <c r="D26" s="2" t="s">
@@ -1900,11 +1909,11 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
+    <row r="27" spans="1:9" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="8" t="s">
         <v>73</v>
       </c>
       <c r="D27" s="2" t="s">
@@ -1923,11 +1932,11 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
+    <row r="28" spans="1:9" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="8" t="s">
         <v>73</v>
       </c>
       <c r="D28" s="2" t="s">
@@ -1946,11 +1955,11 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
+    <row r="29" spans="1:9" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="8" t="s">
         <v>73</v>
       </c>
       <c r="D29" s="2" t="s">
@@ -1969,11 +1978,11 @@
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
+    <row r="30" spans="1:9" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" s="8" t="s">
         <v>73</v>
       </c>
       <c r="D30" s="2" t="s">
@@ -1995,11 +2004,11 @@
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
+    <row r="31" spans="1:9" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C31" s="8" t="s">
         <v>73</v>
       </c>
       <c r="D31" s="2" t="s">
@@ -2018,11 +2027,11 @@
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="10" t="s">
+    <row r="32" spans="1:9" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C32" s="8" t="s">
         <v>73</v>
       </c>
       <c r="D32" s="2" t="s">
@@ -2044,11 +2053,11 @@
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
+    <row r="33" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="8" t="s">
         <v>73</v>
       </c>
       <c r="D33" s="2" t="s">
@@ -2067,11 +2076,11 @@
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
+    <row r="34" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="8" t="s">
         <v>73</v>
       </c>
       <c r="D34" s="2" t="s">
@@ -2093,11 +2102,11 @@
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
+    <row r="35" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C35" s="8" t="s">
         <v>73</v>
       </c>
       <c r="D35" s="2" t="s">
@@ -2119,11 +2128,11 @@
         <v>124</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="10" t="s">
+    <row r="36" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C36" s="8" t="s">
         <v>73</v>
       </c>
       <c r="D36" s="2" t="s">
@@ -2145,11 +2154,11 @@
         <v>124</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="10" t="s">
+    <row r="37" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C37" s="8" t="s">
         <v>73</v>
       </c>
       <c r="D37" s="2" t="s">
@@ -2171,11 +2180,11 @@
         <v>131</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="10" t="s">
+    <row r="38" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="C38" s="8" t="s">
         <v>73</v>
       </c>
       <c r="D38" s="2" t="s">
@@ -2197,11 +2206,11 @@
         <v>131</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="10" t="s">
+    <row r="39" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="C39" s="10" t="s">
+      <c r="C39" s="8" t="s">
         <v>73</v>
       </c>
       <c r="D39" s="2" t="s">
@@ -2223,11 +2232,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="10" t="s">
+    <row r="40" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="C40" s="10" t="s">
+      <c r="C40" s="8" t="s">
         <v>73</v>
       </c>
       <c r="D40" s="2" t="s">
@@ -2249,11 +2258,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="10" t="s">
+    <row r="41" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="C41" s="8" t="s">
         <v>73</v>
       </c>
       <c r="D41" s="2" t="s">
@@ -2275,11 +2284,11 @@
         <v>145</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="10" t="s">
+    <row r="42" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="C42" s="10" t="s">
+      <c r="C42" s="8" t="s">
         <v>73</v>
       </c>
       <c r="D42" s="2" t="s">
@@ -2301,11 +2310,11 @@
         <v>145</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="10" t="s">
+    <row r="43" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="C43" s="10" t="s">
+      <c r="C43" s="8" t="s">
         <v>73</v>
       </c>
       <c r="D43" s="2" t="s">
@@ -2327,11 +2336,11 @@
         <v>152</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="10" t="s">
+    <row r="44" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="C44" s="10" t="s">
+      <c r="C44" s="8" t="s">
         <v>73</v>
       </c>
       <c r="D44" s="2" t="s">
@@ -2353,11 +2362,11 @@
         <v>156</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="10" t="s">
+    <row r="45" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="C45" s="10" t="s">
+      <c r="C45" s="8" t="s">
         <v>73</v>
       </c>
       <c r="D45" s="2" t="s">
@@ -2379,11 +2388,11 @@
         <v>160</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="10" t="s">
+    <row r="46" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="C46" s="10" t="s">
+      <c r="C46" s="8" t="s">
         <v>73</v>
       </c>
       <c r="D46" s="2" t="s">
@@ -2405,11 +2414,11 @@
         <v>164</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="10" t="s">
+    <row r="47" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="C47" s="10" t="s">
+      <c r="C47" s="8" t="s">
         <v>73</v>
       </c>
       <c r="D47" s="2" t="s">
@@ -2431,11 +2440,11 @@
         <v>168</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="10" t="s">
+    <row r="48" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="C48" s="10" t="s">
+      <c r="C48" s="8" t="s">
         <v>170</v>
       </c>
       <c r="D48" s="2" t="s">
@@ -2454,11 +2463,11 @@
         <v>173</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="10" t="s">
+    <row r="49" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="C49" s="10" t="s">
+      <c r="C49" s="8" t="s">
         <v>170</v>
       </c>
       <c r="D49" s="2" t="s">
@@ -2477,11 +2486,11 @@
         <v>173</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="10" t="s">
+    <row r="50" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="C50" s="10" t="s">
+      <c r="C50" s="8" t="s">
         <v>170</v>
       </c>
       <c r="D50" s="2" t="s">
@@ -2500,11 +2509,11 @@
         <v>173</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="10" t="s">
+    <row r="51" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="C51" s="10" t="s">
+      <c r="C51" s="8" t="s">
         <v>170</v>
       </c>
       <c r="D51" s="2" t="s">
@@ -2523,11 +2532,11 @@
         <v>173</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="10" t="s">
+    <row r="52" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="C52" s="10" t="s">
+      <c r="C52" s="8" t="s">
         <v>170</v>
       </c>
       <c r="D52" s="2" t="s">
@@ -2546,11 +2555,11 @@
         <v>173</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="10" t="s">
+    <row r="53" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="C53" s="10" t="s">
+      <c r="C53" s="8" t="s">
         <v>170</v>
       </c>
       <c r="D53" s="2" t="s">
@@ -2569,11 +2578,11 @@
         <v>173</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="10" t="s">
+    <row r="54" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="C54" s="10" t="s">
+      <c r="C54" s="8" t="s">
         <v>170</v>
       </c>
       <c r="D54" s="2" t="s">
@@ -2592,11 +2601,11 @@
         <v>173</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="10" t="s">
+    <row r="55" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="C55" s="10" t="s">
+      <c r="C55" s="8" t="s">
         <v>170</v>
       </c>
       <c r="D55" s="2" t="s">
@@ -2615,11 +2624,11 @@
         <v>173</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="10" t="s">
+    <row r="56" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="C56" s="10" t="s">
+      <c r="C56" s="8" t="s">
         <v>170</v>
       </c>
       <c r="D56" s="2" t="s">
@@ -2638,11 +2647,11 @@
         <v>173</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="10" t="s">
+    <row r="57" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="C57" s="10" t="s">
+      <c r="C57" s="8" t="s">
         <v>170</v>
       </c>
       <c r="D57" s="2" t="s">
@@ -2661,11 +2670,11 @@
         <v>173</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="10" t="s">
+    <row r="58" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="C58" s="10" t="s">
+      <c r="C58" s="8" t="s">
         <v>170</v>
       </c>
       <c r="D58" s="2" t="s">
@@ -2684,11 +2693,11 @@
         <v>173</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="10" t="s">
+    <row r="59" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="C59" s="10" t="s">
+      <c r="C59" s="8" t="s">
         <v>170</v>
       </c>
       <c r="D59" s="2" t="s">
@@ -2707,11 +2716,11 @@
         <v>173</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="10" t="s">
+    <row r="60" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="C60" s="10" t="s">
+      <c r="C60" s="8" t="s">
         <v>170</v>
       </c>
       <c r="D60" s="2" t="s">
@@ -2733,11 +2742,11 @@
         <v>173</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="10" t="s">
+    <row r="61" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="C61" s="10" t="s">
+      <c r="C61" s="8" t="s">
         <v>170</v>
       </c>
       <c r="D61" s="2" t="s">
@@ -2759,11 +2768,11 @@
         <v>173</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="10" t="s">
+    <row r="62" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="C62" s="10" t="s">
+      <c r="C62" s="8" t="s">
         <v>170</v>
       </c>
       <c r="D62" s="2" t="s">
@@ -2785,11 +2794,11 @@
         <v>173</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="10" t="s">
+    <row r="63" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="C63" s="10" t="s">
+      <c r="C63" s="8" t="s">
         <v>170</v>
       </c>
       <c r="D63" s="2" t="s">
@@ -2811,11 +2820,11 @@
         <v>173</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="10" t="s">
+    <row r="64" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="C64" s="10" t="s">
+      <c r="C64" s="8" t="s">
         <v>170</v>
       </c>
       <c r="D64" s="2" t="s">
@@ -2837,11 +2846,11 @@
         <v>173</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="10" t="s">
+    <row r="65" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="C65" s="10" t="s">
+      <c r="C65" s="8" t="s">
         <v>170</v>
       </c>
       <c r="D65" s="2" t="s">
@@ -2866,11 +2875,11 @@
         <v>173</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="10" t="s">
+    <row r="66" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="C66" s="10" t="s">
+      <c r="C66" s="8" t="s">
         <v>170</v>
       </c>
       <c r="D66" s="2" t="s">
@@ -2895,11 +2904,11 @@
         <v>173</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="10" t="s">
+    <row r="67" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="8" t="s">
         <v>230</v>
       </c>
-      <c r="C67" s="10" t="s">
+      <c r="C67" s="8" t="s">
         <v>170</v>
       </c>
       <c r="D67" s="2" t="s">
@@ -2924,11 +2933,11 @@
         <v>173</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="10" t="s">
+    <row r="68" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="C68" s="10" t="s">
+      <c r="C68" s="8" t="s">
         <v>170</v>
       </c>
       <c r="D68" s="2" t="s">
@@ -2953,11 +2962,11 @@
         <v>173</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="10" t="s">
+    <row r="69" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="C69" s="10" t="s">
+      <c r="C69" s="8" t="s">
         <v>170</v>
       </c>
       <c r="D69" s="2" t="s">
@@ -2982,11 +2991,11 @@
         <v>173</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="10" t="s">
+    <row r="70" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="C70" s="10" t="s">
+      <c r="C70" s="8" t="s">
         <v>170</v>
       </c>
       <c r="D70" s="2" t="s">
@@ -3011,11 +3020,11 @@
         <v>173</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="10" t="s">
+    <row r="71" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="C71" s="10" t="s">
+      <c r="C71" s="8" t="s">
         <v>170</v>
       </c>
       <c r="D71" s="2" t="s">
@@ -3040,11 +3049,11 @@
         <v>173</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="10" t="s">
+    <row r="72" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="C72" s="10" t="s">
+      <c r="C72" s="8" t="s">
         <v>170</v>
       </c>
       <c r="D72" s="2" t="s">
@@ -3069,11 +3078,11 @@
         <v>173</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="10" t="s">
+    <row r="73" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="C73" s="10" t="s">
+      <c r="C73" s="8" t="s">
         <v>170</v>
       </c>
       <c r="D73" s="2" t="s">
@@ -3098,11 +3107,11 @@
         <v>173</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="10" t="s">
+    <row r="74" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="8" t="s">
         <v>258</v>
       </c>
-      <c r="C74" s="10" t="s">
+      <c r="C74" s="8" t="s">
         <v>170</v>
       </c>
       <c r="D74" s="2" t="s">
@@ -3127,11 +3136,11 @@
         <v>173</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="10" t="s">
+    <row r="75" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="C75" s="10" t="s">
+      <c r="C75" s="8" t="s">
         <v>170</v>
       </c>
       <c r="D75" s="2" t="s">
@@ -3156,11 +3165,11 @@
         <v>173</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="10" t="s">
+    <row r="76" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="8" t="s">
         <v>265</v>
       </c>
-      <c r="C76" s="10" t="s">
+      <c r="C76" s="8" t="s">
         <v>170</v>
       </c>
       <c r="D76" s="2" t="s">
@@ -3185,724 +3194,724 @@
         <v>173</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" spans="1:10" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="81" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="82" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="83" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="86" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="88" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="89" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="90" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="91" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="92" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="93" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="94" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="95" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="96" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="97" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="98" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="99" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="100" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="101" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="102" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="103" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="104" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="105" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="106" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="107" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="108" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="109" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="110" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="111" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="112" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="113" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="114" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="115" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="116" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="117" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="118" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="119" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="120" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="121" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="124" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="125" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="126" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="127" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="128" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="129" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="130" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="131" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="132" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="133" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="134" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="135" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="136" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="137" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="138" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="139" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="140" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="141" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="142" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="143" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="144" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="145" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="146" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="147" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="148" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="149" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="150" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="151" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="152" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="153" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="154" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="155" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="156" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="157" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="158" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="159" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="160" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="161" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="162" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="163" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="164" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="165" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="166" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="167" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="168" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="169" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="170" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="171" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="172" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="173" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="174" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="175" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="176" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="177" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="178" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="179" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="180" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="181" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="182" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="183" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="184" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="185" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="186" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="187" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="188" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="189" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="190" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="191" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="192" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="193" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="194" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="195" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="196" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="197" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="198" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="199" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="200" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="201" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="202" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="203" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="204" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="205" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="206" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="207" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="208" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="209" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="210" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="211" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="212" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="213" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="214" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="215" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="216" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="217" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="218" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="219" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="220" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="221" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="222" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="223" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="224" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="225" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="226" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="227" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="228" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="229" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="230" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="231" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="232" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="233" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="234" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="235" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="236" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="237" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="238" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="239" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="240" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="241" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="242" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="243" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="244" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="245" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="246" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="247" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="248" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="249" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="250" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="251" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="252" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="253" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="254" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="255" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="256" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="257" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="258" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="259" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="260" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="261" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="262" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="263" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="264" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="265" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="266" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="267" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="268" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="269" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="270" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="271" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="272" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="273" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="274" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="275" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="276" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="277" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="278" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="279" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="280" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="281" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="282" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="283" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="284" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="285" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="286" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="287" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="288" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="289" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="290" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="291" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="292" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="293" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="294" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="295" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="296" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="297" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="298" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="299" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="300" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="301" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="302" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="303" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="304" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="305" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="306" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="307" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="308" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="309" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="310" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="311" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="312" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="313" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="314" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="315" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="316" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="317" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="318" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="319" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="320" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="321" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="322" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="323" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="324" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="325" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="326" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="327" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="328" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="329" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="330" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="331" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="332" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="333" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="334" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="335" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="336" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="337" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="338" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="339" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="340" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="341" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="342" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="343" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="344" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="345" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="346" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="347" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="348" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="349" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="350" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="351" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="352" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="353" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="354" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="355" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="356" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="357" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="358" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="359" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="360" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="361" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="362" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="363" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="364" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="365" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="366" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="367" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="368" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="369" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="370" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="371" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="372" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="373" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="374" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="375" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="376" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="377" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="378" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="379" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="380" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="381" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="382" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="383" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="384" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="385" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="386" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="387" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="388" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="389" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="390" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="391" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="392" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="393" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="394" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="395" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="396" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="397" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="398" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="399" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="400" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="401" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="402" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="403" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="404" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="405" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="406" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="407" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="408" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="409" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="410" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="411" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="412" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="413" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="414" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="415" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="416" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="417" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="418" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="419" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="420" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="421" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="422" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="423" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="424" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="425" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="426" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="427" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="428" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="429" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="430" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="431" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="432" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="433" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="434" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="435" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="436" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="437" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="438" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="439" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="440" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="441" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="442" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="443" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="444" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="445" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="446" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="447" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="448" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="449" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="450" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="451" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="452" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="453" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="454" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="455" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="456" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="457" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="458" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="459" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="460" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="461" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="462" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="463" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="464" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="465" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="466" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="467" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="468" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="469" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="470" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="471" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="472" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="473" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="474" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="475" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="476" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="477" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="478" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="479" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="480" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="481" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="482" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="483" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="484" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="485" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="486" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="487" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="488" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="489" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="490" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="491" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="492" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="493" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="494" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="495" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="496" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="497" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="498" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="499" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="500" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="501" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="502" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="503" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="504" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="505" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="506" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="507" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="508" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="509" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="510" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="511" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="512" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="513" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="514" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="515" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="516" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="517" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="518" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="519" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="520" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="521" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="522" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="523" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="524" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="525" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="526" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="527" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="528" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="529" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="530" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="531" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="532" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="533" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="534" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="535" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="536" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="537" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="538" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="539" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="540" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="541" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="542" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="543" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="544" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="545" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="546" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="547" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="548" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="549" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="550" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="551" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="552" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="553" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="554" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="555" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="556" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="557" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="558" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="559" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="560" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="561" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="562" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="563" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="564" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="565" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="566" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="567" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="568" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="569" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="570" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="571" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="572" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="573" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="574" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="575" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="576" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="577" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="578" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="579" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="580" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="581" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="582" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="583" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="584" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="585" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="586" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="587" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="588" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="589" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="590" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="591" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="592" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="593" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="594" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="595" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="596" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="597" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="598" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="599" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="600" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="601" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="602" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="603" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="604" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="605" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="606" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="607" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="608" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="609" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="610" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="611" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="612" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="613" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="614" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="615" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="616" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="617" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="618" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="619" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="620" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="621" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="622" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="623" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="624" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="625" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="626" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="627" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="628" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="629" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="630" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="631" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="632" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="633" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="634" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="635" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="636" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="637" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="638" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="639" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="640" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="641" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="642" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="643" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="644" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="645" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="646" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="647" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="648" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="649" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="650" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="651" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="652" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="653" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="654" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="655" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="656" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="657" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="658" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="659" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="660" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="661" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="662" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="663" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="664" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="665" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="666" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="667" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="668" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="669" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="670" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="671" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="672" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="673" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="674" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="675" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="676" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="677" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="678" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="679" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="680" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="681" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="682" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="683" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="684" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="685" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="686" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="687" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="688" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="689" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="690" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="691" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="692" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="693" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="694" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="695" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="696" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="697" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="698" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="699" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="700" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="701" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="702" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="703" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="704" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="705" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="706" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="707" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="708" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="709" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="710" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="711" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="712" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="713" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="714" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="715" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="716" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="717" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="718" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="719" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="720" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="721" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="722" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="723" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="724" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="725" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="726" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="727" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="728" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="729" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="730" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="731" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="732" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="733" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="734" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="735" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="736" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="737" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="738" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="739" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="740" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="741" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="742" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="743" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="744" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="745" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="746" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="747" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="748" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="749" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="750" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="751" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="752" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="753" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="754" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="755" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="756" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="757" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="758" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="759" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="760" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="761" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="762" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="763" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="764" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="765" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="766" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="767" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="768" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="769" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="770" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="771" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="772" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="773" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="774" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="775" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="776" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="777" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="778" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="779" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="780" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="781" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="782" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="783" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="784" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="785" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="786" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="787" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="788" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="789" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="790" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="791" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="792" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="793" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="794" ht="12.3" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="1:10" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="141" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="142" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="164" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="182" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="183" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="184" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="186" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="187" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="188" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="189" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="190" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="191" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="192" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="205" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="206" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="207" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="208" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="209" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="224" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="225" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="226" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="227" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="228" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="229" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="230" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="231" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="232" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="233" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="234" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="235" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="236" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="237" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="238" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="239" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="240" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="241" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="242" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="243" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="245" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="246" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="248" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="251" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="254" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="255" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="256" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="257" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="259" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="260" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="275" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="276" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="277" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="278" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="279" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="281" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="282" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="283" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="290" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="291" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="292" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="293" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="294" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="295" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="296" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="297" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="298" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="299" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="300" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="301" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="302" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="303" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="304" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="305" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="306" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="307" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="308" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="309" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="310" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="311" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="312" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="313" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="314" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="315" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="316" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="317" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="318" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="319" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="320" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="321" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="322" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="323" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="324" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="325" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="326" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="327" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="328" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="329" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="330" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="331" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="332" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="333" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="334" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="335" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="336" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="337" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="338" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="339" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="340" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="341" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="342" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="343" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="344" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="345" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="346" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="347" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="348" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="349" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="350" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="351" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="352" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="353" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="354" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="355" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="356" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="357" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="358" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="359" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="360" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="361" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="362" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="363" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="364" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="365" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="366" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="367" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="368" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="369" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="370" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="371" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="372" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="373" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="374" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="375" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="376" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="377" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="378" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="379" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="380" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="381" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="382" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="383" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="384" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="385" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="386" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="387" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="388" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="389" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="390" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="391" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="392" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="393" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="394" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="395" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="396" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="397" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="398" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="399" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="400" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="401" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="402" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="403" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="404" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="405" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="406" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="407" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="408" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="409" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="410" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="411" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="412" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="413" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="414" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="415" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="416" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="417" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="418" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="419" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="420" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="421" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="422" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="423" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="424" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="425" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="426" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="427" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="428" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="429" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="430" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="431" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="432" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="433" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="434" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="435" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="436" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="437" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="438" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="439" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="440" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="441" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="442" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="443" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="444" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="445" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="446" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="447" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="448" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="449" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="450" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="451" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="452" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="453" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="454" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="455" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="456" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="457" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="458" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="459" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="460" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="461" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="462" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="463" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="464" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="465" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="466" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="467" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="468" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="469" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="470" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="471" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="472" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="473" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="474" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="475" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="476" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="477" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="478" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="479" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="480" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="481" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="482" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="483" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="484" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="485" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="486" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="487" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="488" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="489" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="490" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="491" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="492" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="493" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="494" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="495" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="496" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="497" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="498" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="499" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="500" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="501" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="502" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="503" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="504" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="505" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="506" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="507" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="508" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="509" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="510" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="511" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="512" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="513" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="514" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="515" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="516" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="517" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="518" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="519" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="520" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="521" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="522" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="523" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="524" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="525" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="526" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="527" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="528" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="529" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="530" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="531" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="532" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="533" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="534" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="535" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="536" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="537" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="538" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="539" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="540" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="541" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="542" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="543" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="544" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="545" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="546" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="547" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="548" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="549" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="550" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="551" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="552" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="553" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="554" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="555" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="556" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="557" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="558" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="559" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="560" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="561" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="562" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="563" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="564" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="565" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="566" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="567" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="568" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="569" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="570" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="571" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="572" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="573" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="574" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="575" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="576" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="577" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="578" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="579" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="580" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="581" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="582" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="583" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="584" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="585" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="586" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="587" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="588" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="589" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="590" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="591" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="592" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="593" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="594" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="595" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="596" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="597" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="598" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="599" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="600" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="601" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="602" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="603" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="604" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="605" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="606" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="607" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="608" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="609" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="610" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="611" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="612" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="613" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="614" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="615" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="616" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="617" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="618" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="619" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="620" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="621" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="622" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="623" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="624" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="625" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="626" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="627" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="628" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="629" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="630" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="631" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="632" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="633" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="634" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="635" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="636" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="637" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="638" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="639" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="640" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="641" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="642" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="643" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="644" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="645" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="646" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="647" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="648" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="649" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="650" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="651" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="652" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="653" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="654" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="655" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="656" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="657" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="658" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="659" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="660" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="661" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="662" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="663" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="664" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="665" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="666" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="667" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="668" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="669" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="670" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="671" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="672" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="673" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="674" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="675" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="676" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="677" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="678" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="679" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="680" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="681" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="682" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="683" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="684" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="685" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="686" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="687" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="688" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="689" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="690" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="691" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="692" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="693" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="694" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="695" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="696" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="697" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="698" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="699" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="700" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="701" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="702" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="703" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="704" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="705" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="706" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="707" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="708" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="709" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="710" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="711" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="712" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="713" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="714" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="715" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="716" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="717" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="718" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="719" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="720" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="721" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="722" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="723" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="724" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="725" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="726" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="727" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="728" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="729" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="730" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="731" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="732" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="733" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="734" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="735" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="736" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="737" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="738" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="739" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="740" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="741" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="742" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="743" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="744" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="745" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="746" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="747" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="748" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="749" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="750" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="751" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="752" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="753" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="754" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="755" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="756" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="757" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="758" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="759" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="760" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="761" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="762" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="763" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="764" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="765" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="766" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="767" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="768" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="769" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="770" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="771" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="772" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="773" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="774" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="775" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="776" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="777" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="778" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="779" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="780" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="781" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="782" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="783" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="784" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="785" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="786" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="787" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="788" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="789" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="790" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="791" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="792" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="793" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="794" ht="12.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:J1"/>
@@ -3924,12 +3933,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3937,12 +3946,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>